<commit_message>
Revert level1.csv for check storyid
</commit_message>
<xml_diff>
--- a/20190829 작업 필요 리스트업.xlsx
+++ b/20190829 작업 필요 리스트업.xlsx
@@ -107,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +117,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,7 +156,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -158,6 +164,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,7 +473,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -513,16 +522,16 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>